<commit_message>
Update Definitions main classes & Origins.xlsx
</commit_message>
<xml_diff>
--- a/Thematic Workshop 2/Definitions main classes & Origins.xlsx
+++ b/Thematic Workshop 2/Definitions main classes & Origins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haleydtk\Documents\GitHub\OSLOthema-airAndWater\Thematic Workshop 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43206A0C-F70B-464A-AF56-98306AE3441B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD5B13B-BF0A-4E0B-B80C-94AF65E18107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="-15885" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Class</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>FIWARE</t>
+  </si>
+  <si>
+    <t>Metadata is data that contains information about data.</t>
+  </si>
+  <si>
+    <t>Spatially defined part of the Object to be observed and representative of that Object</t>
   </si>
 </sst>
 </file>
@@ -485,7 +491,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -543,7 +549,9 @@
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
@@ -563,7 +571,9 @@
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>

</xml_diff>